<commit_message>
sum ok fixed ^$ regex to replace was the fix
</commit_message>
<xml_diff>
--- a/Sondage.xlsx
+++ b/Sondage.xlsx
@@ -9493,16 +9493,16 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0.1742</v>
+        <v>2.12</v>
       </c>
       <c r="U2" t="n">
-        <v>320.5419</v>
+        <v>37.59</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>20370.31</v>
+        <v>240.1</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
@@ -9578,19 +9578,19 @@
         <v>21509</v>
       </c>
       <c r="S3" t="n">
-        <v>0.12</v>
+        <v>1.2</v>
       </c>
       <c r="T3" t="n">
-        <v>0.123</v>
+        <v>1.5</v>
       </c>
       <c r="U3" t="n">
-        <v>190.3029</v>
+        <v>22.29</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>19440.53</v>
+        <v>239.3</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -9666,22 +9666,22 @@
         <v>76043</v>
       </c>
       <c r="S4" t="n">
-        <v>130.3416</v>
+        <v>16.56</v>
       </c>
       <c r="T4" t="n">
-        <v>20.20441901</v>
+        <v>4.4591</v>
       </c>
       <c r="U4" t="n">
-        <v>160.173312</v>
+        <v>18.042</v>
       </c>
       <c r="V4" t="n">
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>6280.2417</v>
+        <v>90.57000000000001</v>
       </c>
       <c r="X4" t="n">
-        <v>1050.2513</v>
+        <v>17.63</v>
       </c>
     </row>
     <row r="5">
@@ -9754,22 +9754,22 @@
         <v>26008</v>
       </c>
       <c r="S5" t="n">
-        <v>3100.1817</v>
+        <v>41.97000000000001</v>
       </c>
       <c r="T5" t="n">
-        <v>30.304803</v>
+        <v>6.483</v>
       </c>
       <c r="U5" t="n">
-        <v>2280.392808</v>
+        <v>52.188</v>
       </c>
       <c r="V5" t="n">
-        <v>10.000004</v>
+        <v>1.004</v>
       </c>
       <c r="W5" t="n">
-        <v>10290.36</v>
+        <v>132.6</v>
       </c>
       <c r="X5" t="n">
-        <v>60.19090000000001</v>
+        <v>7.99</v>
       </c>
     </row>
     <row r="6">
@@ -9842,22 +9842,22 @@
         <v>2016</v>
       </c>
       <c r="S6" t="n">
-        <v>11270.4605</v>
+        <v>141.65</v>
       </c>
       <c r="T6" t="n">
-        <v>70.37371215</v>
+        <v>11.0835</v>
       </c>
       <c r="U6" t="n">
-        <v>2210.332001</v>
+        <v>44.501</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>5310.1934</v>
+        <v>83.23999999999999</v>
       </c>
       <c r="X6" t="n">
-        <v>170.3914</v>
+        <v>21.04</v>
       </c>
     </row>
     <row r="7">
@@ -9930,22 +9930,22 @@
         <v>12755</v>
       </c>
       <c r="S7" t="n">
-        <v>5070.3404</v>
+        <v>60.44</v>
       </c>
       <c r="T7" t="n">
-        <v>50.15269999999999</v>
+        <v>6.77</v>
       </c>
       <c r="U7" t="n">
-        <v>2170.391003</v>
+        <v>41.003</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0009</v>
+        <v>0.09</v>
       </c>
       <c r="W7" t="n">
-        <v>8480.4112</v>
+        <v>132.22</v>
       </c>
       <c r="X7" t="n">
-        <v>4080.1313</v>
+        <v>49.43</v>
       </c>
     </row>
     <row r="8">
@@ -10018,22 +10018,22 @@
         <v>39228</v>
       </c>
       <c r="S8" t="n">
-        <v>1090.3006</v>
+        <v>22.06</v>
       </c>
       <c r="T8" t="n">
-        <v>0.17431105</v>
+        <v>2.1415</v>
       </c>
       <c r="U8" t="n">
-        <v>1140.234006</v>
+        <v>26.706</v>
       </c>
       <c r="V8" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="W8" t="n">
-        <v>7360.363200000001</v>
+        <v>109.92</v>
       </c>
       <c r="X8" t="n">
-        <v>80.16079999999999</v>
+        <v>9.68</v>
       </c>
     </row>
     <row r="9">
@@ -10106,22 +10106,22 @@
         <v>30750</v>
       </c>
       <c r="S9" t="n">
-        <v>4200.27</v>
+        <v>62.7</v>
       </c>
       <c r="T9" t="n">
-        <v>30.363203</v>
+        <v>6.923000000000001</v>
       </c>
       <c r="U9" t="n">
-        <v>260.2427</v>
+        <v>28.66999999999999</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="W9" t="n">
-        <v>6350.4617</v>
+        <v>99.77</v>
       </c>
       <c r="X9" t="n">
-        <v>110.3213</v>
+        <v>14.33</v>
       </c>
     </row>
     <row r="10">
@@ -10197,16 +10197,16 @@
         <v>0</v>
       </c>
       <c r="T10" t="n">
-        <v>0.06370000000000001</v>
+        <v>0.97</v>
       </c>
       <c r="U10" t="n">
-        <v>220.4351</v>
+        <v>26.81</v>
       </c>
       <c r="V10" t="n">
         <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>23420.25</v>
+        <v>274.5</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -10282,22 +10282,22 @@
         <v>11024</v>
       </c>
       <c r="S11" t="n">
-        <v>9180.252</v>
+        <v>110.7</v>
       </c>
       <c r="T11" t="n">
-        <v>30.274808</v>
+        <v>6.188</v>
       </c>
       <c r="U11" t="n">
-        <v>3260.443807</v>
+        <v>60.787</v>
       </c>
       <c r="V11" t="n">
         <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>8530.391299999999</v>
+        <v>137.03</v>
       </c>
       <c r="X11" t="n">
-        <v>2240.202</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="12">
@@ -10370,19 +10370,19 @@
         <v>36310</v>
       </c>
       <c r="S12" t="n">
-        <v>0.09</v>
+        <v>0.9</v>
       </c>
       <c r="T12" t="n">
-        <v>0.1627</v>
+        <v>1.87</v>
       </c>
       <c r="U12" t="n">
-        <v>250.2738</v>
+        <v>28.08</v>
       </c>
       <c r="V12" t="n">
         <v>0</v>
       </c>
       <c r="W12" t="n">
-        <v>18550.46</v>
+        <v>239.6</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -10458,22 +10458,22 @@
         <v>13440</v>
       </c>
       <c r="S13" t="n">
-        <v>220.3007</v>
+        <v>25.07</v>
       </c>
       <c r="T13" t="n">
-        <v>20.223706</v>
+        <v>4.576000000000001</v>
       </c>
       <c r="U13" t="n">
-        <v>30.212207</v>
+        <v>5.327</v>
       </c>
       <c r="V13" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="W13" t="n">
-        <v>4280.4718</v>
+        <v>72.88000000000001</v>
       </c>
       <c r="X13" t="n">
-        <v>100.3802</v>
+        <v>13.82</v>
       </c>
     </row>
     <row r="14">
@@ -10546,22 +10546,22 @@
         <v>13720</v>
       </c>
       <c r="S14" t="n">
-        <v>5130.2211</v>
+        <v>65.31</v>
       </c>
       <c r="T14" t="n">
-        <v>40.283611</v>
+        <v>7.170999999999999</v>
       </c>
       <c r="U14" t="n">
-        <v>6260.2907</v>
+        <v>88.97</v>
       </c>
       <c r="V14" t="n">
         <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>4190.354</v>
+        <v>62.9</v>
       </c>
       <c r="X14" t="n">
-        <v>1180.2213</v>
+        <v>30.33</v>
       </c>
     </row>
     <row r="15">
@@ -10634,22 +10634,22 @@
         <v>19666</v>
       </c>
       <c r="S15" t="n">
-        <v>13230.3721</v>
+        <v>156.91</v>
       </c>
       <c r="T15" t="n">
-        <v>20.314725</v>
+        <v>5.594999999999999</v>
       </c>
       <c r="U15" t="n">
-        <v>1140.26160002</v>
+        <v>26.7602</v>
       </c>
       <c r="V15" t="n">
-        <v>10.04</v>
+        <v>1.4</v>
       </c>
       <c r="W15" t="n">
-        <v>400.4253</v>
+        <v>44.73</v>
       </c>
       <c r="X15" t="n">
-        <v>270.3812</v>
+        <v>30.92</v>
       </c>
     </row>
     <row r="16">
@@ -10722,22 +10722,22 @@
         <v>6254</v>
       </c>
       <c r="S16" t="n">
-        <v>15280.4402</v>
+        <v>182.42</v>
       </c>
       <c r="T16" t="n">
-        <v>10.206212</v>
+        <v>3.632</v>
       </c>
       <c r="U16" t="n">
-        <v>2370.30170202</v>
+        <v>60.17220000000001</v>
       </c>
       <c r="V16" t="n">
-        <v>10.04</v>
+        <v>1.4</v>
       </c>
       <c r="W16" t="n">
-        <v>4330.2228</v>
+        <v>75.48</v>
       </c>
       <c r="X16" t="n">
-        <v>130.3912</v>
+        <v>17.02</v>
       </c>
     </row>
     <row r="17">
@@ -10810,22 +10810,22 @@
         <v>25971</v>
       </c>
       <c r="S17" t="n">
-        <v>3150.1909</v>
+        <v>46.99</v>
       </c>
       <c r="T17" t="n">
-        <v>4150.234503</v>
+        <v>57.753</v>
       </c>
       <c r="U17" t="n">
-        <v>2120.1125</v>
+        <v>33.35</v>
       </c>
       <c r="V17" t="n">
-        <v>20.12</v>
+        <v>3.2</v>
       </c>
       <c r="W17" t="n">
-        <v>5180.6422</v>
+        <v>74.62</v>
       </c>
       <c r="X17" t="n">
-        <v>80.12</v>
+        <v>9.200000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -10898,22 +10898,22 @@
         <v>24004</v>
       </c>
       <c r="S18" t="n">
-        <v>5220.3514</v>
+        <v>75.63999999999999</v>
       </c>
       <c r="T18" t="n">
-        <v>10.134919</v>
+        <v>2.809</v>
       </c>
       <c r="U18" t="n">
-        <v>2160.392502</v>
+        <v>40.15199999999999</v>
       </c>
       <c r="V18" t="n">
         <v>0</v>
       </c>
       <c r="W18" t="n">
-        <v>2280.4228</v>
+        <v>52.48</v>
       </c>
       <c r="X18" t="n">
-        <v>140.2406</v>
+        <v>16.46</v>
       </c>
     </row>
     <row r="19">
@@ -10986,22 +10986,22 @@
         <v>11109</v>
       </c>
       <c r="S19" t="n">
-        <v>13250.2811</v>
+        <v>157.91</v>
       </c>
       <c r="T19" t="n">
-        <v>20.27401</v>
+        <v>5.109999999999999</v>
       </c>
       <c r="U19" t="n">
-        <v>1240.2938</v>
+        <v>37.28000000000001</v>
       </c>
       <c r="V19" t="n">
         <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>2220.4423</v>
+        <v>46.63</v>
       </c>
       <c r="X19" t="n">
-        <v>130.3927</v>
+        <v>17.17</v>
       </c>
     </row>
     <row r="20">
@@ -11074,22 +11074,22 @@
         <v>20254</v>
       </c>
       <c r="S20" t="n">
-        <v>12170.3013</v>
+        <v>140.13</v>
       </c>
       <c r="T20" t="n">
-        <v>10.10312213</v>
+        <v>2.3333</v>
       </c>
       <c r="U20" t="n">
-        <v>160.233605</v>
+        <v>18.665</v>
       </c>
       <c r="V20" t="n">
-        <v>0.0001</v>
+        <v>0.01</v>
       </c>
       <c r="W20" t="n">
-        <v>5240.481799999999</v>
+        <v>78.98</v>
       </c>
       <c r="X20" t="n">
-        <v>170.1519</v>
+        <v>18.69</v>
       </c>
     </row>
     <row r="21">
@@ -11162,22 +11162,22 @@
         <v>32028</v>
       </c>
       <c r="S21" t="n">
-        <v>8190.200800000001</v>
+        <v>101.08</v>
       </c>
       <c r="T21" t="n">
-        <v>10.23441</v>
+        <v>3.75</v>
       </c>
       <c r="U21" t="n">
-        <v>2230.3638</v>
+        <v>46.98</v>
       </c>
       <c r="V21" t="n">
         <v>0</v>
       </c>
       <c r="W21" t="n">
-        <v>2190.3518</v>
+        <v>42.67999999999999</v>
       </c>
       <c r="X21" t="n">
-        <v>130.3627</v>
+        <v>16.87</v>
       </c>
     </row>
     <row r="22">
@@ -11250,22 +11250,22 @@
         <v>36039</v>
       </c>
       <c r="S22" t="n">
-        <v>13200.35</v>
+        <v>153.5</v>
       </c>
       <c r="T22" t="n">
-        <v>10.32341909</v>
+        <v>4.559899999999999</v>
       </c>
       <c r="U22" t="n">
-        <v>3140.350903</v>
+        <v>47.593</v>
       </c>
       <c r="V22" t="n">
         <v>0</v>
       </c>
       <c r="W22" t="n">
-        <v>8190.3819</v>
+        <v>102.99</v>
       </c>
       <c r="X22" t="n">
-        <v>110.1516</v>
+        <v>12.66</v>
       </c>
     </row>
     <row r="23">
@@ -11341,16 +11341,16 @@
         <v>0</v>
       </c>
       <c r="T23" t="n">
-        <v>0.1037</v>
+        <v>1.37</v>
       </c>
       <c r="U23" t="n">
-        <v>150.4033</v>
+        <v>19.33000000000001</v>
       </c>
       <c r="V23" t="n">
         <v>0</v>
       </c>
       <c r="W23" t="n">
-        <v>19590.41</v>
+        <v>253.1</v>
       </c>
       <c r="X23" t="n">
         <v>0</v>
@@ -11426,22 +11426,22 @@
         <v>25901</v>
       </c>
       <c r="S24" t="n">
-        <v>6340.331700000001</v>
+        <v>97.47000000000001</v>
       </c>
       <c r="T24" t="n">
-        <v>30.35451301</v>
+        <v>6.9631</v>
       </c>
       <c r="U24" t="n">
-        <v>2070.23230002</v>
+        <v>29.5302</v>
       </c>
       <c r="V24" t="n">
-        <v>10.04</v>
+        <v>1.4</v>
       </c>
       <c r="W24" t="n">
-        <v>1310.3038</v>
+        <v>44.38</v>
       </c>
       <c r="X24" t="n">
-        <v>250.3118</v>
+        <v>28.27999999999999</v>
       </c>
     </row>
     <row r="25">
@@ -11514,22 +11514,22 @@
         <v>20330</v>
       </c>
       <c r="S25" t="n">
-        <v>14110.3402</v>
+        <v>154.42</v>
       </c>
       <c r="T25" t="n">
-        <v>10.152818</v>
+        <v>2.798</v>
       </c>
       <c r="U25" t="n">
-        <v>90.08190902000001</v>
+        <v>9.9992</v>
       </c>
       <c r="V25" t="n">
-        <v>20.13</v>
+        <v>3.3</v>
       </c>
       <c r="W25" t="n">
-        <v>2230.332</v>
+        <v>46.5</v>
       </c>
       <c r="X25" t="n">
-        <v>110.1702</v>
+        <v>12.72</v>
       </c>
     </row>
     <row r="26">
@@ -11602,22 +11602,22 @@
         <v>17640</v>
       </c>
       <c r="S26" t="n">
-        <v>6200.2218</v>
+        <v>82.38</v>
       </c>
       <c r="T26" t="n">
-        <v>20.18250901</v>
+        <v>4.0591</v>
       </c>
       <c r="U26" t="n">
-        <v>3210.472502</v>
+        <v>55.952</v>
       </c>
       <c r="V26" t="n">
-        <v>0.000602</v>
+        <v>0.062</v>
       </c>
       <c r="W26" t="n">
-        <v>4390.4215</v>
+        <v>83.35000000000001</v>
       </c>
       <c r="X26" t="n">
-        <v>4260.2005</v>
+        <v>68.05</v>
       </c>
     </row>
     <row r="27">
@@ -11690,22 +11690,22 @@
         <v>19122</v>
       </c>
       <c r="S27" t="n">
-        <v>1210.3319</v>
+        <v>34.48999999999999</v>
       </c>
       <c r="T27" t="n">
-        <v>10.17441205</v>
+        <v>3.152499999999999</v>
       </c>
       <c r="U27" t="n">
-        <v>2090.254119</v>
+        <v>31.929</v>
       </c>
       <c r="V27" t="n">
         <v>0</v>
       </c>
       <c r="W27" t="n">
-        <v>6260.4631</v>
+        <v>90.91</v>
       </c>
       <c r="X27" t="n">
-        <v>70.1724</v>
+        <v>8.94</v>
       </c>
     </row>
     <row r="28">
@@ -11778,22 +11778,22 @@
         <v>8373</v>
       </c>
       <c r="S28" t="n">
-        <v>8060.3718</v>
+        <v>89.88000000000001</v>
       </c>
       <c r="T28" t="n">
-        <v>80.19361701999999</v>
+        <v>10.2772</v>
       </c>
       <c r="U28" t="n">
-        <v>3150.2708</v>
+        <v>47.78</v>
       </c>
       <c r="V28" t="n">
         <v>0</v>
       </c>
       <c r="W28" t="n">
-        <v>8350.300499999999</v>
+        <v>118.05</v>
       </c>
       <c r="X28" t="n">
-        <v>1160.2105</v>
+        <v>28.15</v>
       </c>
     </row>
     <row r="29">
@@ -11866,22 +11866,22 @@
         <v>9816</v>
       </c>
       <c r="S29" t="n">
-        <v>1100.2007</v>
+        <v>22.07</v>
       </c>
       <c r="T29" t="n">
-        <v>40.192405</v>
+        <v>6.145</v>
       </c>
       <c r="U29" t="n">
-        <v>2210.3226050108</v>
+        <v>44.46518</v>
       </c>
       <c r="V29" t="n">
         <v>0</v>
       </c>
       <c r="W29" t="n">
-        <v>5390.431</v>
+        <v>93.40000000000001</v>
       </c>
       <c r="X29" t="n">
-        <v>1040.4005</v>
+        <v>18.05</v>
       </c>
     </row>
     <row r="30">
@@ -11954,22 +11954,22 @@
         <v>11168</v>
       </c>
       <c r="S30" t="n">
-        <v>3100.1618</v>
+        <v>41.78</v>
       </c>
       <c r="T30" t="n">
-        <v>10.364103</v>
+        <v>5.013</v>
       </c>
       <c r="U30" t="n">
-        <v>90.2655</v>
+        <v>12.15</v>
       </c>
       <c r="V30" t="n">
         <v>0</v>
       </c>
       <c r="W30" t="n">
-        <v>9330.361699999999</v>
+        <v>126.77</v>
       </c>
       <c r="X30" t="n">
-        <v>160.182</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
@@ -12042,22 +12042,22 @@
         <v>25410</v>
       </c>
       <c r="S31" t="n">
-        <v>2220.4722</v>
+        <v>46.92000000000001</v>
       </c>
       <c r="T31" t="n">
-        <v>40.173219</v>
+        <v>6.039</v>
       </c>
       <c r="U31" t="n">
-        <v>140.363917</v>
+        <v>18.007</v>
       </c>
       <c r="V31" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="W31" t="n">
-        <v>2470.5232</v>
+        <v>72.52</v>
       </c>
       <c r="X31" t="n">
-        <v>190.4119</v>
+        <v>23.29</v>
       </c>
     </row>
     <row r="32">
@@ -12130,19 +12130,19 @@
         <v>36600</v>
       </c>
       <c r="S32" t="n">
-        <v>0.06</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="T32" t="n">
-        <v>0.1433</v>
+        <v>1.73</v>
       </c>
       <c r="U32" t="n">
-        <v>270.3233</v>
+        <v>30.53</v>
       </c>
       <c r="V32" t="n">
         <v>0</v>
       </c>
       <c r="W32" t="n">
-        <v>18540.53</v>
+        <v>239.3</v>
       </c>
       <c r="X32" t="n">
         <v>0</v>
@@ -12218,22 +12218,22 @@
         <v>20201</v>
       </c>
       <c r="S33" t="n">
-        <v>3240.271999999999</v>
+        <v>56.9</v>
       </c>
       <c r="T33" t="n">
-        <v>40.102122</v>
+        <v>5.231999999999999</v>
       </c>
       <c r="U33" t="n">
-        <v>100.224105</v>
+        <v>12.615</v>
       </c>
       <c r="V33" t="n">
         <v>0</v>
       </c>
       <c r="W33" t="n">
-        <v>5170.2343</v>
+        <v>69.72999999999999</v>
       </c>
       <c r="X33" t="n">
-        <v>5180.252</v>
+        <v>70.69999999999999</v>
       </c>
     </row>
     <row r="34">
@@ -12306,22 +12306,22 @@
         <v>31113</v>
       </c>
       <c r="S34" t="n">
-        <v>6160.4519</v>
+        <v>80.69</v>
       </c>
       <c r="T34" t="n">
-        <v>50.29431</v>
+        <v>8.340000000000002</v>
       </c>
       <c r="U34" t="n">
-        <v>3160.383699999999</v>
+        <v>50.17</v>
       </c>
       <c r="V34" t="n">
-        <v>60.2305</v>
+        <v>8.35</v>
       </c>
       <c r="W34" t="n">
-        <v>5480.5641</v>
+        <v>104.01</v>
       </c>
       <c r="X34" t="n">
-        <v>260.3204</v>
+        <v>29.24</v>
       </c>
     </row>
     <row r="35">
@@ -12394,22 +12394,22 @@
         <v>22011</v>
       </c>
       <c r="S35" t="n">
-        <v>4170.4826</v>
+        <v>62.06</v>
       </c>
       <c r="T35" t="n">
-        <v>1090.31201308</v>
+        <v>22.3138</v>
       </c>
       <c r="U35" t="n">
-        <v>6290.3522</v>
+        <v>92.71999999999998</v>
       </c>
       <c r="V35" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="W35" t="n">
-        <v>5220.392608000001</v>
+        <v>76.16800000000001</v>
       </c>
       <c r="X35" t="n">
-        <v>100.241</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="36">
@@ -12482,22 +12482,22 @@
         <v>17030</v>
       </c>
       <c r="S36" t="n">
-        <v>11230.1911</v>
+        <v>135.01</v>
       </c>
       <c r="T36" t="n">
-        <v>10.273203</v>
+        <v>4.023</v>
       </c>
       <c r="U36" t="n">
-        <v>2310.4022</v>
+        <v>55.22</v>
       </c>
       <c r="V36" t="n">
         <v>0</v>
       </c>
       <c r="W36" t="n">
-        <v>220.3223</v>
+        <v>25.43</v>
       </c>
       <c r="X36" t="n">
-        <v>60.3521</v>
+        <v>9.710000000000001</v>
       </c>
     </row>
     <row r="37">
@@ -12570,22 +12570,22 @@
         <v>32115</v>
       </c>
       <c r="S37" t="n">
-        <v>5090.2408</v>
+        <v>61.48</v>
       </c>
       <c r="T37" t="n">
-        <v>10.23281002</v>
+        <v>3.5902</v>
       </c>
       <c r="U37" t="n">
-        <v>1150.26290002</v>
+        <v>27.8902</v>
       </c>
       <c r="V37" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="W37" t="n">
-        <v>5420.441503</v>
+        <v>96.553</v>
       </c>
       <c r="X37" t="n">
-        <v>2180.2908</v>
+        <v>40.98</v>
       </c>
     </row>
     <row r="38">
@@ -12658,22 +12658,22 @@
         <v>31081</v>
       </c>
       <c r="S38" t="n">
-        <v>11210.1911</v>
+        <v>133.01</v>
       </c>
       <c r="T38" t="n">
-        <v>10.28321</v>
+        <v>4.13</v>
       </c>
       <c r="U38" t="n">
-        <v>2270.3931</v>
+        <v>51.21</v>
       </c>
       <c r="V38" t="n">
         <v>0</v>
       </c>
       <c r="W38" t="n">
-        <v>1210.4221</v>
+        <v>35.41</v>
       </c>
       <c r="X38" t="n">
-        <v>50.4614</v>
+        <v>9.74</v>
       </c>
     </row>
     <row r="39">
@@ -12746,22 +12746,22 @@
         <v>23588</v>
       </c>
       <c r="S39" t="n">
-        <v>6330.4515</v>
+        <v>97.65000000000001</v>
       </c>
       <c r="T39" t="n">
-        <v>0.276709</v>
+        <v>3.379</v>
       </c>
       <c r="U39" t="n">
-        <v>3340.4728</v>
+        <v>68.98</v>
       </c>
       <c r="V39" t="n">
         <v>0</v>
       </c>
       <c r="W39" t="n">
-        <v>1510.3737</v>
+        <v>65.07000000000001</v>
       </c>
       <c r="X39" t="n">
-        <v>90.3707</v>
+        <v>12.77</v>
       </c>
     </row>
     <row r="40">
@@ -12834,22 +12834,22 @@
         <v>12114</v>
       </c>
       <c r="S40" t="n">
-        <v>11250.23</v>
+        <v>137.3</v>
       </c>
       <c r="T40" t="n">
-        <v>30.264506</v>
+        <v>6.055999999999999</v>
       </c>
       <c r="U40" t="n">
-        <v>5340.422299999999</v>
+        <v>88.42999999999999</v>
       </c>
       <c r="V40" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="W40" t="n">
-        <v>4610.4145</v>
+        <v>105.55</v>
       </c>
       <c r="X40" t="n">
-        <v>2240.2609</v>
+        <v>46.69</v>
       </c>
     </row>
     <row r="41">
@@ -12922,22 +12922,22 @@
         <v>20141</v>
       </c>
       <c r="S41" t="n">
-        <v>130.3835</v>
+        <v>17.15</v>
       </c>
       <c r="T41" t="n">
-        <v>10.042215</v>
+        <v>1.635</v>
       </c>
       <c r="U41" t="n">
-        <v>100.112122</v>
+        <v>11.332</v>
       </c>
       <c r="V41" t="n">
-        <v>0.0405</v>
+        <v>0.45</v>
       </c>
       <c r="W41" t="n">
-        <v>1330.2733</v>
+        <v>46.02999999999999</v>
       </c>
       <c r="X41" t="n">
-        <v>130.19</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="42">
@@ -13010,22 +13010,22 @@
         <v>19639</v>
       </c>
       <c r="S42" t="n">
-        <v>4210.2209</v>
+        <v>63.29000000000001</v>
       </c>
       <c r="T42" t="n">
-        <v>0.163622</v>
+        <v>1.982</v>
       </c>
       <c r="U42" t="n">
-        <v>1160.3026</v>
+        <v>29.26000000000001</v>
       </c>
       <c r="V42" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="W42" t="n">
-        <v>8330.412600000001</v>
+        <v>117.36</v>
       </c>
       <c r="X42" t="n">
-        <v>80.08</v>
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="43">
@@ -13098,22 +13098,22 @@
         <v>17325</v>
       </c>
       <c r="S43" t="n">
-        <v>8170.251099999999</v>
+        <v>99.61</v>
       </c>
       <c r="T43" t="n">
-        <v>20.27351</v>
+        <v>5.06</v>
       </c>
       <c r="U43" t="n">
-        <v>1260.3038</v>
+        <v>39.38</v>
       </c>
       <c r="V43" t="n">
         <v>0</v>
       </c>
       <c r="W43" t="n">
-        <v>2170.3916</v>
+        <v>41.06</v>
       </c>
       <c r="X43" t="n">
-        <v>90.402</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="44">
@@ -13186,22 +13186,22 @@
         <v>36036</v>
       </c>
       <c r="S44" t="n">
-        <v>1200.3518</v>
+        <v>33.68</v>
       </c>
       <c r="T44" t="n">
-        <v>10.12171002</v>
+        <v>2.3802</v>
       </c>
       <c r="U44" t="n">
-        <v>2200.222101</v>
+        <v>42.411</v>
       </c>
       <c r="V44" t="n">
-        <v>0.000309</v>
+        <v>0.039</v>
       </c>
       <c r="W44" t="n">
-        <v>4470.282299999999</v>
+        <v>90.03</v>
       </c>
       <c r="X44" t="n">
-        <v>1150.2015</v>
+        <v>27.15</v>
       </c>
     </row>
     <row r="45">
@@ -13274,22 +13274,22 @@
         <v>19641</v>
       </c>
       <c r="S45" t="n">
-        <v>5150.2619</v>
+        <v>67.78999999999999</v>
       </c>
       <c r="T45" t="n">
-        <v>30.133217</v>
+        <v>4.637</v>
       </c>
       <c r="U45" t="n">
-        <v>2170.293003</v>
+        <v>40.203</v>
       </c>
       <c r="V45" t="n">
-        <v>0.021006</v>
+        <v>0.306</v>
       </c>
       <c r="W45" t="n">
-        <v>5340.3717</v>
+        <v>87.86999999999999</v>
       </c>
       <c r="X45" t="n">
-        <v>30.1007</v>
+        <v>4.07</v>
       </c>
     </row>
     <row r="46">
@@ -13362,22 +13362,22 @@
         <v>23410</v>
       </c>
       <c r="S46" t="n">
-        <v>130.3822</v>
+        <v>17.02</v>
       </c>
       <c r="T46" t="n">
-        <v>30.274118</v>
+        <v>6.128</v>
       </c>
       <c r="U46" t="n">
-        <v>280.304711</v>
+        <v>31.481</v>
       </c>
       <c r="V46" t="n">
         <v>0</v>
       </c>
       <c r="W46" t="n">
-        <v>6320.502100000001</v>
+        <v>97.21000000000001</v>
       </c>
       <c r="X46" t="n">
-        <v>210.371</v>
+        <v>24.8</v>
       </c>
     </row>
     <row r="47">
@@ -13450,22 +13450,22 @@
         <v>17030</v>
       </c>
       <c r="S47" t="n">
-        <v>13210.2508</v>
+        <v>153.58</v>
       </c>
       <c r="T47" t="n">
-        <v>20.223007</v>
+        <v>4.507</v>
       </c>
       <c r="U47" t="n">
-        <v>2390.3531</v>
+        <v>62.80999999999999</v>
       </c>
       <c r="V47" t="n">
         <v>0</v>
       </c>
       <c r="W47" t="n">
-        <v>2150.4321</v>
+        <v>39.51000000000001</v>
       </c>
       <c r="X47" t="n">
-        <v>90.32199999999999</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="48">
@@ -13538,22 +13538,22 @@
         <v>17100</v>
       </c>
       <c r="S48" t="n">
-        <v>13180.2806</v>
+        <v>150.86</v>
       </c>
       <c r="T48" t="n">
-        <v>20.21281</v>
+        <v>4.390000000000001</v>
       </c>
       <c r="U48" t="n">
-        <v>2310.353</v>
+        <v>54.8</v>
       </c>
       <c r="V48" t="n">
         <v>0</v>
       </c>
       <c r="W48" t="n">
-        <v>2180.4015</v>
+        <v>42.15000000000001</v>
       </c>
       <c r="X48" t="n">
-        <v>70.42139999999999</v>
+        <v>11.34</v>
       </c>
     </row>
     <row r="49">
@@ -13626,22 +13626,22 @@
         <v>9231</v>
       </c>
       <c r="S49" t="n">
-        <v>4150.4317</v>
+        <v>59.46999999999999</v>
       </c>
       <c r="T49" t="n">
-        <v>90.094808</v>
+        <v>10.388</v>
       </c>
       <c r="U49" t="n">
-        <v>3320.4522</v>
+        <v>66.72</v>
       </c>
       <c r="V49" t="n">
         <v>0</v>
       </c>
       <c r="W49" t="n">
-        <v>8190.3714</v>
+        <v>102.84</v>
       </c>
       <c r="X49" t="n">
-        <v>1180.1604</v>
+        <v>29.64</v>
       </c>
     </row>
     <row r="50">
@@ -13714,22 +13714,22 @@
         <v>20055</v>
       </c>
       <c r="S50" t="n">
-        <v>1100.2403</v>
+        <v>22.43</v>
       </c>
       <c r="T50" t="n">
-        <v>10.1427110303</v>
+        <v>2.68133</v>
       </c>
       <c r="U50" t="n">
-        <v>80.09150000000001</v>
+        <v>9.049999999999999</v>
       </c>
       <c r="V50" t="n">
-        <v>20.07</v>
+        <v>2.7</v>
       </c>
       <c r="W50" t="n">
-        <v>3300.2317</v>
+        <v>62.47</v>
       </c>
       <c r="X50" t="n">
-        <v>90.19</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="51">
@@ -13802,22 +13802,22 @@
         <v>25629</v>
       </c>
       <c r="S51" t="n">
-        <v>6080.1809</v>
+        <v>69.89</v>
       </c>
       <c r="T51" t="n">
-        <v>20.31271701</v>
+        <v>5.3871</v>
       </c>
       <c r="U51" t="n">
-        <v>90.31261599999999</v>
+        <v>12.376</v>
       </c>
       <c r="V51" t="n">
-        <v>0.04</v>
+        <v>0.4</v>
       </c>
       <c r="W51" t="n">
-        <v>6180.3415</v>
+        <v>81.55</v>
       </c>
       <c r="X51" t="n">
-        <v>1110.33</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="52">
@@ -13890,22 +13890,22 @@
         <v>25901</v>
       </c>
       <c r="S52" t="n">
-        <v>11220.4102</v>
+        <v>136.12</v>
       </c>
       <c r="T52" t="n">
-        <v>30.3928</v>
+        <v>7.18</v>
       </c>
       <c r="U52" t="n">
-        <v>4200.3208</v>
+        <v>63.27999999999999</v>
       </c>
       <c r="V52" t="n">
         <v>0</v>
       </c>
       <c r="W52" t="n">
-        <v>300.2741</v>
+        <v>33.11</v>
       </c>
       <c r="X52" t="n">
-        <v>180.2914</v>
+        <v>21.04</v>
       </c>
     </row>
     <row r="53">
@@ -13978,22 +13978,22 @@
         <v>25584</v>
       </c>
       <c r="S53" t="n">
-        <v>2190.2912</v>
+        <v>42.02</v>
       </c>
       <c r="T53" t="n">
-        <v>90.353703</v>
+        <v>12.873</v>
       </c>
       <c r="U53" t="n">
-        <v>130.2726</v>
+        <v>15.96</v>
       </c>
       <c r="V53" t="n">
-        <v>1060.090105</v>
+        <v>16.915</v>
       </c>
       <c r="W53" t="n">
-        <v>6300.461600000001</v>
+        <v>94.76000000000001</v>
       </c>
       <c r="X53" t="n">
-        <v>170.2612</v>
+        <v>19.72</v>
       </c>
     </row>
     <row r="54">
@@ -14066,22 +14066,22 @@
         <v>16742</v>
       </c>
       <c r="S54" t="n">
-        <v>8220.3117</v>
+        <v>105.27</v>
       </c>
       <c r="T54" t="n">
-        <v>30.082624</v>
+        <v>4.084000000000001</v>
       </c>
       <c r="U54" t="n">
-        <v>250.412704</v>
+        <v>29.374</v>
       </c>
       <c r="V54" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="W54" t="n">
-        <v>5340.351500000001</v>
+        <v>87.64999999999999</v>
       </c>
       <c r="X54" t="n">
-        <v>180.3409</v>
+        <v>21.49</v>
       </c>
     </row>
     <row r="55">
@@ -14154,22 +14154,22 @@
         <v>25126</v>
       </c>
       <c r="S55" t="n">
-        <v>2210.4018</v>
+        <v>45.18</v>
       </c>
       <c r="T55" t="n">
-        <v>120.1849</v>
+        <v>14.29</v>
       </c>
       <c r="U55" t="n">
-        <v>2200.2428</v>
+        <v>42.68</v>
       </c>
       <c r="V55" t="n">
-        <v>0.0103</v>
+        <v>0.13</v>
       </c>
       <c r="W55" t="n">
-        <v>6400.501600000001</v>
+        <v>105.16</v>
       </c>
       <c r="X55" t="n">
-        <v>70.16250000000001</v>
+        <v>8.85</v>
       </c>
     </row>
     <row r="56">
@@ -14242,22 +14242,22 @@
         <v>8001</v>
       </c>
       <c r="S56" t="n">
-        <v>7160.3212</v>
+        <v>89.32000000000001</v>
       </c>
       <c r="T56" t="n">
-        <v>20.16361906</v>
+        <v>3.9796</v>
       </c>
       <c r="U56" t="n">
-        <v>1240.372906</v>
+        <v>37.996</v>
       </c>
       <c r="V56" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="W56" t="n">
-        <v>3250.5127</v>
+        <v>60.37</v>
       </c>
       <c r="X56" t="n">
-        <v>1260.4201</v>
+        <v>40.21</v>
       </c>
     </row>
     <row r="57">
@@ -14330,22 +14330,22 @@
         <v>19591</v>
       </c>
       <c r="S57" t="n">
-        <v>12260.1804</v>
+        <v>147.84</v>
       </c>
       <c r="T57" t="n">
-        <v>10.193812</v>
+        <v>3.292</v>
       </c>
       <c r="U57" t="n">
-        <v>1190.3344</v>
+        <v>32.73999999999999</v>
       </c>
       <c r="V57" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="W57" t="n">
-        <v>3340.4035</v>
+        <v>68.35000000000001</v>
       </c>
       <c r="X57" t="n">
-        <v>1080.1415</v>
+        <v>19.55</v>
       </c>
     </row>
     <row r="58">
@@ -14418,22 +14418,22 @@
         <v>20518</v>
       </c>
       <c r="S58" t="n">
-        <v>5290.310201089999</v>
+        <v>82.1219</v>
       </c>
       <c r="T58" t="n">
-        <v>80.20500801999999</v>
+        <v>10.5082</v>
       </c>
       <c r="U58" t="n">
-        <v>1220.2624</v>
+        <v>34.84</v>
       </c>
       <c r="V58" t="n">
-        <v>0.050004</v>
+        <v>0.504</v>
       </c>
       <c r="W58" t="n">
-        <v>6450.122200000001</v>
+        <v>106.42</v>
       </c>
       <c r="X58" t="n">
-        <v>6210.240000090001</v>
+        <v>83.40090000000001</v>
       </c>
     </row>
     <row r="59">
@@ -14506,22 +14506,22 @@
         <v>13720</v>
       </c>
       <c r="S59" t="n">
-        <v>8190.3516</v>
+        <v>102.66</v>
       </c>
       <c r="T59" t="n">
-        <v>30.124311</v>
+        <v>4.641</v>
       </c>
       <c r="U59" t="n">
-        <v>2230.503</v>
+        <v>48.3</v>
       </c>
       <c r="V59" t="n">
         <v>0</v>
       </c>
       <c r="W59" t="n">
-        <v>2440.3741</v>
+        <v>68.11</v>
       </c>
       <c r="X59" t="n">
-        <v>250.2708</v>
+        <v>27.78</v>
       </c>
     </row>
     <row r="60">
@@ -14594,22 +14594,22 @@
         <v>10064</v>
       </c>
       <c r="S60" t="n">
-        <v>3110.222</v>
+        <v>43.4</v>
       </c>
       <c r="T60" t="n">
-        <v>40.2932040705</v>
+        <v>7.22475</v>
       </c>
       <c r="U60" t="n">
-        <v>130.313708</v>
+        <v>16.478</v>
       </c>
       <c r="V60" t="n">
         <v>0</v>
       </c>
       <c r="W60" t="n">
-        <v>6460.4422</v>
+        <v>110.62</v>
       </c>
       <c r="X60" t="n">
-        <v>240.2918</v>
+        <v>27.08</v>
       </c>
     </row>
     <row r="61">
@@ -14682,22 +14682,22 @@
         <v>11217</v>
       </c>
       <c r="S61" t="n">
-        <v>3160.3024</v>
+        <v>49.23999999999999</v>
       </c>
       <c r="T61" t="n">
-        <v>70.30260699999999</v>
+        <v>10.267</v>
       </c>
       <c r="U61" t="n">
-        <v>1190.132501</v>
+        <v>30.551</v>
       </c>
       <c r="V61" t="n">
-        <v>0.0709</v>
+        <v>0.79</v>
       </c>
       <c r="W61" t="n">
-        <v>8370.2325</v>
+        <v>119.55</v>
       </c>
       <c r="X61" t="n">
-        <v>70.151</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="62">
@@ -14770,22 +14770,22 @@
         <v>30791</v>
       </c>
       <c r="S62" t="n">
-        <v>2170.3407</v>
+        <v>40.47</v>
       </c>
       <c r="T62" t="n">
-        <v>50.22293005</v>
+        <v>7.520499999999999</v>
       </c>
       <c r="U62" t="n">
-        <v>210.363509</v>
+        <v>24.959</v>
       </c>
       <c r="V62" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="W62" t="n">
-        <v>6200.592499999999</v>
+        <v>86.15000000000001</v>
       </c>
       <c r="X62" t="n">
-        <v>110.2205</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="63">
@@ -14858,22 +14858,22 @@
         <v>13176</v>
       </c>
       <c r="S63" t="n">
-        <v>2170.4308</v>
+        <v>41.38</v>
       </c>
       <c r="T63" t="n">
-        <v>30.13300905</v>
+        <v>4.609500000000001</v>
       </c>
       <c r="U63" t="n">
-        <v>1170.202408</v>
+        <v>29.248</v>
       </c>
       <c r="V63" t="n">
         <v>0</v>
       </c>
       <c r="W63" t="n">
-        <v>7350.501899999999</v>
+        <v>110.19</v>
       </c>
       <c r="X63" t="n">
-        <v>3270.180499999999</v>
+        <v>58.85</v>
       </c>
     </row>
     <row r="64">
@@ -14946,22 +14946,22 @@
         <v>8300</v>
       </c>
       <c r="S64" t="n">
-        <v>3300.3717</v>
+        <v>63.87</v>
       </c>
       <c r="T64" t="n">
-        <v>50.08211005</v>
+        <v>6.0205</v>
       </c>
       <c r="U64" t="n">
-        <v>1300.282718</v>
+        <v>43.088</v>
       </c>
       <c r="V64" t="n">
-        <v>0.06030000000000001</v>
+        <v>0.63</v>
       </c>
       <c r="W64" t="n">
-        <v>4270.4222</v>
+        <v>71.42</v>
       </c>
       <c r="X64" t="n">
-        <v>60.27</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="65">
@@ -15034,22 +15034,22 @@
         <v>23850</v>
       </c>
       <c r="S65" t="n">
-        <v>10310.4105</v>
+        <v>135.15</v>
       </c>
       <c r="T65" t="n">
-        <v>20.364708</v>
+        <v>6.078</v>
       </c>
       <c r="U65" t="n">
-        <v>2240.27220002</v>
+        <v>46.92019999999999</v>
       </c>
       <c r="V65" t="n">
-        <v>10.04</v>
+        <v>1.4</v>
       </c>
       <c r="W65" t="n">
-        <v>2300.2331</v>
+        <v>52.61</v>
       </c>
       <c r="X65" t="n">
-        <v>160.5005</v>
+        <v>21.05</v>
       </c>
     </row>
     <row r="66">
@@ -15122,22 +15122,22 @@
         <v>20535</v>
       </c>
       <c r="S66" t="n">
-        <v>1070.2316</v>
+        <v>19.46</v>
       </c>
       <c r="T66" t="n">
-        <v>30.2033</v>
+        <v>5.33</v>
       </c>
       <c r="U66" t="n">
-        <v>5240.262106000001</v>
+        <v>76.816</v>
       </c>
       <c r="V66" t="n">
-        <v>0.0009</v>
+        <v>0.09</v>
       </c>
       <c r="W66" t="n">
-        <v>8290.27</v>
+        <v>111.7</v>
       </c>
       <c r="X66" t="n">
-        <v>1150.1005</v>
+        <v>26.05</v>
       </c>
     </row>
     <row r="67">
@@ -15210,19 +15210,19 @@
         <v>36206</v>
       </c>
       <c r="S67" t="n">
-        <v>0.12</v>
+        <v>1.2</v>
       </c>
       <c r="T67" t="n">
-        <v>0.1241</v>
+        <v>1.61</v>
       </c>
       <c r="U67" t="n">
-        <v>200.4432</v>
+        <v>24.72</v>
       </c>
       <c r="V67" t="n">
         <v>0</v>
       </c>
       <c r="W67" t="n">
-        <v>18500.52</v>
+        <v>235.2</v>
       </c>
       <c r="X67" t="n">
         <v>0</v>
@@ -15298,22 +15298,22 @@
         <v>30300</v>
       </c>
       <c r="S68" t="n">
-        <v>3090.1925</v>
+        <v>41.15000000000001</v>
       </c>
       <c r="T68" t="n">
-        <v>70.354714</v>
+        <v>10.984</v>
       </c>
       <c r="U68" t="n">
-        <v>2220.351713</v>
+        <v>45.68299999999999</v>
       </c>
       <c r="V68" t="n">
-        <v>8.080000000000001e-06</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="W68" t="n">
-        <v>4410.382299999999</v>
+        <v>85.03</v>
       </c>
       <c r="X68" t="n">
-        <v>120.4111</v>
+        <v>16.21</v>
       </c>
     </row>
     <row r="69">
@@ -15386,22 +15386,22 @@
         <v>31018</v>
       </c>
       <c r="S69" t="n">
-        <v>9270.3614</v>
+        <v>120.74</v>
       </c>
       <c r="T69" t="n">
-        <v>20.24370805</v>
+        <v>4.7785</v>
       </c>
       <c r="U69" t="n">
-        <v>1250.202113</v>
+        <v>37.223</v>
       </c>
       <c r="V69" t="n">
         <v>0</v>
       </c>
       <c r="W69" t="n">
-        <v>2360.2516</v>
+        <v>58.66</v>
       </c>
       <c r="X69" t="n">
-        <v>2120.2907</v>
+        <v>34.97000000000001</v>
       </c>
     </row>
     <row r="70">
@@ -15474,22 +15474,22 @@
         <v>20299</v>
       </c>
       <c r="S70" t="n">
-        <v>5290.3412</v>
+        <v>82.52000000000001</v>
       </c>
       <c r="T70" t="n">
-        <v>50.33281400000001</v>
+        <v>8.593999999999999</v>
       </c>
       <c r="U70" t="n">
-        <v>1230.2431</v>
+        <v>35.71</v>
       </c>
       <c r="V70" t="n">
-        <v>20.13</v>
+        <v>3.3</v>
       </c>
       <c r="W70" t="n">
-        <v>4250.3423</v>
+        <v>68.63</v>
       </c>
       <c r="X70" t="n">
-        <v>80.41079999999999</v>
+        <v>12.18</v>
       </c>
     </row>
     <row r="71">
@@ -15562,22 +15562,22 @@
         <v>12064</v>
       </c>
       <c r="S71" t="n">
-        <v>120.4626</v>
+        <v>16.86</v>
       </c>
       <c r="T71" t="n">
-        <v>4140.36250806</v>
+        <v>57.85860000000001</v>
       </c>
       <c r="U71" t="n">
-        <v>4380.402314999999</v>
+        <v>82.24499999999999</v>
       </c>
       <c r="V71" t="n">
         <v>0</v>
       </c>
       <c r="W71" t="n">
-        <v>9330.521799999999</v>
+        <v>128.38</v>
       </c>
       <c r="X71" t="n">
-        <v>200.3426</v>
+        <v>23.66</v>
       </c>
     </row>
     <row r="72">
@@ -15650,22 +15650,22 @@
         <v>16404</v>
       </c>
       <c r="S72" t="n">
-        <v>7190.280300000001</v>
+        <v>91.83</v>
       </c>
       <c r="T72" t="n">
-        <v>30.09382807</v>
+        <v>4.3087</v>
       </c>
       <c r="U72" t="n">
-        <v>4250.261200020001</v>
+        <v>67.72019999999999</v>
       </c>
       <c r="V72" t="n">
-        <v>10.04</v>
+        <v>1.4</v>
       </c>
       <c r="W72" t="n">
-        <v>6210.493000000001</v>
+        <v>86.2</v>
       </c>
       <c r="X72" t="n">
-        <v>100.1606</v>
+        <v>11.66</v>
       </c>
     </row>
     <row r="73">
@@ -15738,22 +15738,22 @@
         <v>11109</v>
       </c>
       <c r="S73" t="n">
-        <v>13260.3011</v>
+        <v>159.11</v>
       </c>
       <c r="T73" t="n">
-        <v>20.333903</v>
+        <v>5.693</v>
       </c>
       <c r="U73" t="n">
-        <v>1200.3129</v>
+        <v>33.39</v>
       </c>
       <c r="V73" t="n">
         <v>0</v>
       </c>
       <c r="W73" t="n">
-        <v>1230.3723</v>
+        <v>36.93</v>
       </c>
       <c r="X73" t="n">
-        <v>100.4327</v>
+        <v>14.57</v>
       </c>
     </row>
     <row r="74">
@@ -15826,22 +15826,22 @@
         <v>3000</v>
       </c>
       <c r="S74" t="n">
-        <v>6260.3907</v>
+        <v>89.97</v>
       </c>
       <c r="T74" t="n">
-        <v>0.22450705</v>
+        <v>2.6575</v>
       </c>
       <c r="U74" t="n">
-        <v>100.3128</v>
+        <v>13.38</v>
       </c>
       <c r="V74" t="n">
-        <v>0.040307</v>
+        <v>0.437</v>
       </c>
       <c r="W74" t="n">
-        <v>5330.440799999999</v>
+        <v>87.48</v>
       </c>
       <c r="X74" t="n">
-        <v>2120.2221</v>
+        <v>34.41</v>
       </c>
     </row>
     <row r="75">
@@ -15914,22 +15914,22 @@
         <v>25917</v>
       </c>
       <c r="S75" t="n">
-        <v>11210.1911</v>
+        <v>133.01</v>
       </c>
       <c r="T75" t="n">
-        <v>10.28321</v>
+        <v>4.13</v>
       </c>
       <c r="U75" t="n">
-        <v>1320.3631</v>
+        <v>45.91</v>
       </c>
       <c r="V75" t="n">
         <v>0</v>
       </c>
       <c r="W75" t="n">
-        <v>1210.4221</v>
+        <v>35.41</v>
       </c>
       <c r="X75" t="n">
-        <v>50.4614</v>
+        <v>9.74</v>
       </c>
     </row>
     <row r="76">
@@ -16002,22 +16002,22 @@
         <v>31026</v>
       </c>
       <c r="S76" t="n">
-        <v>8140.3313</v>
+        <v>97.43000000000001</v>
       </c>
       <c r="T76" t="n">
-        <v>60.29451</v>
+        <v>9.360000000000001</v>
       </c>
       <c r="U76" t="n">
-        <v>4120.363708999999</v>
+        <v>55.979</v>
       </c>
       <c r="V76" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="W76" t="n">
-        <v>3390.572799999999</v>
+        <v>74.97999999999999</v>
       </c>
       <c r="X76" t="n">
-        <v>200.3722</v>
+        <v>23.92</v>
       </c>
     </row>
     <row r="77">
@@ -16090,22 +16090,22 @@
         <v>23496</v>
       </c>
       <c r="S77" t="n">
-        <v>9200.420700000001</v>
+        <v>114.27</v>
       </c>
       <c r="T77" t="n">
-        <v>10.11492</v>
+        <v>2.61</v>
       </c>
       <c r="U77" t="n">
-        <v>4410.451902000001</v>
+        <v>85.69200000000001</v>
       </c>
       <c r="V77" t="n">
         <v>0</v>
       </c>
       <c r="W77" t="n">
-        <v>6190.471799999999</v>
+        <v>83.88</v>
       </c>
       <c r="X77" t="n">
-        <v>1100.2407</v>
+        <v>22.47</v>
       </c>
     </row>
     <row r="78">
@@ -16178,22 +16178,22 @@
         <v>20031</v>
       </c>
       <c r="S78" t="n">
-        <v>6070.0914</v>
+        <v>68.04000000000001</v>
       </c>
       <c r="T78" t="n">
-        <v>1020.15101208</v>
+        <v>13.6128</v>
       </c>
       <c r="U78" t="n">
-        <v>1120.152601</v>
+        <v>23.761</v>
       </c>
       <c r="V78" t="n">
         <v>0</v>
       </c>
       <c r="W78" t="n">
-        <v>11180.2609</v>
+        <v>130.69</v>
       </c>
       <c r="X78" t="n">
-        <v>1040.03</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="79">
@@ -16266,22 +16266,22 @@
         <v>7025</v>
       </c>
       <c r="S79" t="n">
-        <v>2190.191699999999</v>
+        <v>41.07</v>
       </c>
       <c r="T79" t="n">
-        <v>40.193709</v>
+        <v>6.279000000000001</v>
       </c>
       <c r="U79" t="n">
-        <v>4250.3018</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="V79" t="n">
         <v>0</v>
       </c>
       <c r="W79" t="n">
-        <v>2580.413300000001</v>
+        <v>82.43000000000001</v>
       </c>
       <c r="X79" t="n">
-        <v>210.1303</v>
+        <v>22.33</v>
       </c>
     </row>
     <row r="80">
@@ -16354,22 +16354,22 @@
         <v>18005</v>
       </c>
       <c r="S80" t="n">
-        <v>2160.2511</v>
+        <v>38.61000000000001</v>
       </c>
       <c r="T80" t="n">
-        <v>60.334515</v>
+        <v>9.765000000000002</v>
       </c>
       <c r="U80" t="n">
-        <v>1120.3521</v>
+        <v>25.71</v>
       </c>
       <c r="V80" t="n">
         <v>0</v>
       </c>
       <c r="W80" t="n">
-        <v>7470.312</v>
+        <v>120.3</v>
       </c>
       <c r="X80" t="n">
-        <v>2290.1904</v>
+        <v>50.94</v>
       </c>
     </row>
     <row r="81">
@@ -16442,22 +16442,22 @@
         <v>20111</v>
       </c>
       <c r="S81" t="n">
-        <v>10210.2615</v>
+        <v>123.75</v>
       </c>
       <c r="T81" t="n">
-        <v>20.234034</v>
+        <v>4.734</v>
       </c>
       <c r="U81" t="n">
-        <v>1210.243809</v>
+        <v>33.78899999999999</v>
       </c>
       <c r="V81" t="n">
-        <v>10.050309</v>
+        <v>1.539</v>
       </c>
       <c r="W81" t="n">
-        <v>5340.673</v>
+        <v>91</v>
       </c>
       <c r="X81" t="n">
-        <v>160.4519</v>
+        <v>20.69</v>
       </c>
     </row>
     <row r="82">
@@ -16530,22 +16530,22 @@
         <v>20326</v>
       </c>
       <c r="S82" t="n">
-        <v>1030.2014</v>
+        <v>15.14</v>
       </c>
       <c r="T82" t="n">
-        <v>50.34282204000001</v>
+        <v>8.702399999999999</v>
       </c>
       <c r="U82" t="n">
-        <v>2230.383310999999</v>
+        <v>47.14100000000001</v>
       </c>
       <c r="V82" t="n">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="W82" t="n">
-        <v>14380.3514</v>
+        <v>181.64</v>
       </c>
       <c r="X82" t="n">
-        <v>130.2217</v>
+        <v>15.37</v>
       </c>
     </row>
     <row r="83">
@@ -16618,19 +16618,19 @@
         <v>36101</v>
       </c>
       <c r="S83" t="n">
-        <v>0.11</v>
+        <v>1.1</v>
       </c>
       <c r="T83" t="n">
-        <v>0.1544</v>
+        <v>1.94</v>
       </c>
       <c r="U83" t="n">
-        <v>320.5147</v>
+        <v>37.57</v>
       </c>
       <c r="V83" t="n">
         <v>0</v>
       </c>
       <c r="W83" t="n">
-        <v>15620.51</v>
+        <v>217.1</v>
       </c>
       <c r="X83" t="n">
         <v>0</v>
@@ -16706,22 +16706,22 @@
         <v>12763</v>
       </c>
       <c r="S84" t="n">
-        <v>3150.3917</v>
+        <v>49.07000000000001</v>
       </c>
       <c r="T84" t="n">
-        <v>10.18371806</v>
+        <v>3.1886</v>
       </c>
       <c r="U84" t="n">
-        <v>3260.3026</v>
+        <v>59.26</v>
       </c>
       <c r="V84" t="n">
         <v>0</v>
       </c>
       <c r="W84" t="n">
-        <v>7250.412300000001</v>
+        <v>99.32999999999998</v>
       </c>
       <c r="X84" t="n">
-        <v>1040.2504</v>
+        <v>16.54</v>
       </c>
     </row>
     <row r="85">
@@ -16794,22 +16794,22 @@
         <v>25154</v>
       </c>
       <c r="S85" t="n">
-        <v>7220.2917</v>
+        <v>95.07000000000001</v>
       </c>
       <c r="T85" t="n">
-        <v>70.22231604999999</v>
+        <v>9.4465</v>
       </c>
       <c r="U85" t="n">
-        <v>140.283602</v>
+        <v>17.162</v>
       </c>
       <c r="V85" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="W85" t="n">
-        <v>3290.2622</v>
+        <v>61.82</v>
       </c>
       <c r="X85" t="n">
-        <v>120.2513</v>
+        <v>14.63</v>
       </c>
     </row>
     <row r="86">
@@ -16882,22 +16882,22 @@
         <v>8015</v>
       </c>
       <c r="S86" t="n">
-        <v>3280.470600000001</v>
+        <v>62.76</v>
       </c>
       <c r="T86" t="n">
-        <v>20.195314</v>
+        <v>4.444</v>
       </c>
       <c r="U86" t="n">
-        <v>3370.463207</v>
+        <v>71.92699999999999</v>
       </c>
       <c r="V86" t="n">
         <v>0</v>
       </c>
       <c r="W86" t="n">
-        <v>5400.462</v>
+        <v>94.8</v>
       </c>
       <c r="X86" t="n">
-        <v>4050.170903</v>
+        <v>46.793</v>
       </c>
     </row>
     <row r="87">
@@ -16970,22 +16970,22 @@
         <v>20284</v>
       </c>
       <c r="S87" t="n">
-        <v>1200.3221</v>
+        <v>33.41</v>
       </c>
       <c r="T87" t="n">
-        <v>30.164423</v>
+        <v>5.063000000000001</v>
       </c>
       <c r="U87" t="n">
-        <v>1150.202912</v>
+        <v>27.302</v>
       </c>
       <c r="V87" t="n">
         <v>0</v>
       </c>
       <c r="W87" t="n">
-        <v>4310.442</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="X87" t="n">
-        <v>130.311603</v>
+        <v>16.263</v>
       </c>
     </row>
     <row r="88">
@@ -17058,22 +17058,22 @@
         <v>26239</v>
       </c>
       <c r="S88" t="n">
-        <v>6210.320699999999</v>
+        <v>84.27</v>
       </c>
       <c r="T88" t="n">
-        <v>10.23151</v>
+        <v>3.46</v>
       </c>
       <c r="U88" t="n">
-        <v>50.27210100000001</v>
+        <v>7.911</v>
       </c>
       <c r="V88" t="n">
-        <v>0.000302</v>
+        <v>0.032</v>
       </c>
       <c r="W88" t="n">
-        <v>3260.3415</v>
+        <v>59.55</v>
       </c>
       <c r="X88" t="n">
-        <v>30.1415</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="89">
@@ -17146,22 +17146,22 @@
         <v>15018</v>
       </c>
       <c r="S89" t="n">
-        <v>17250.27</v>
+        <v>197.7</v>
       </c>
       <c r="T89" t="n">
-        <v>0.131915</v>
+        <v>1.505</v>
       </c>
       <c r="U89" t="n">
-        <v>1160.213908</v>
+        <v>28.498</v>
       </c>
       <c r="V89" t="n">
-        <v>20.1603</v>
+        <v>3.63</v>
       </c>
       <c r="W89" t="n">
-        <v>3240.363612</v>
+        <v>57.972</v>
       </c>
       <c r="X89" t="n">
-        <v>250.410607</v>
+        <v>29.16699999999999</v>
       </c>
     </row>
     <row r="90">
@@ -17234,22 +17234,22 @@
         <v>19692</v>
       </c>
       <c r="S90" t="n">
-        <v>4160.3107</v>
+        <v>59.17000000000001</v>
       </c>
       <c r="T90" t="n">
-        <v>30.2030000705</v>
+        <v>5.300750000000001</v>
       </c>
       <c r="U90" t="n">
-        <v>4190.382302999999</v>
+        <v>63.03299999999999</v>
       </c>
       <c r="V90" t="n">
-        <v>0.0801</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="W90" t="n">
-        <v>10400.3613</v>
+        <v>143.73</v>
       </c>
       <c r="X90" t="n">
-        <v>170.2005</v>
+        <v>19.05</v>
       </c>
     </row>
     <row r="91">
@@ -17322,22 +17322,22 @@
         <v>19044</v>
       </c>
       <c r="S91" t="n">
-        <v>11200.2918</v>
+        <v>133.08</v>
       </c>
       <c r="T91" t="n">
-        <v>20.104231</v>
+        <v>3.451</v>
       </c>
       <c r="U91" t="n">
-        <v>2160.23090202</v>
+        <v>38.3922</v>
       </c>
       <c r="V91" t="n">
-        <v>10.04</v>
+        <v>1.4</v>
       </c>
       <c r="W91" t="n">
-        <v>5180.532300000001</v>
+        <v>73.53</v>
       </c>
       <c r="X91" t="n">
-        <v>140.1803</v>
+        <v>15.83</v>
       </c>
     </row>
     <row r="92">
@@ -17410,19 +17410,19 @@
         <v>21503</v>
       </c>
       <c r="S92" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="T92" t="n">
-        <v>0.1943</v>
+        <v>2.33</v>
       </c>
       <c r="U92" t="n">
-        <v>270.4839</v>
+        <v>32.19</v>
       </c>
       <c r="V92" t="n">
         <v>0</v>
       </c>
       <c r="W92" t="n">
-        <v>19610.44</v>
+        <v>255.4</v>
       </c>
       <c r="X92" t="n">
         <v>0</v>
@@ -17498,22 +17498,22 @@
         <v>12743</v>
       </c>
       <c r="S93" t="n">
-        <v>3150.3109</v>
+        <v>48.19</v>
       </c>
       <c r="T93" t="n">
-        <v>20.193109</v>
+        <v>4.218999999999999</v>
       </c>
       <c r="U93" t="n">
-        <v>3250.271402</v>
+        <v>57.842</v>
       </c>
       <c r="V93" t="n">
         <v>0</v>
       </c>
       <c r="W93" t="n">
-        <v>3260.3522</v>
+        <v>59.72</v>
       </c>
       <c r="X93" t="n">
-        <v>130.1406</v>
+        <v>14.46</v>
       </c>
     </row>
     <row r="94">
@@ -17586,22 +17586,22 @@
         <v>11115</v>
       </c>
       <c r="S94" t="n">
-        <v>4100.2304</v>
+        <v>52.34</v>
       </c>
       <c r="T94" t="n">
-        <v>10.19512703</v>
+        <v>3.4373</v>
       </c>
       <c r="U94" t="n">
-        <v>4150.311900000001</v>
+        <v>58.29</v>
       </c>
       <c r="V94" t="n">
         <v>0</v>
       </c>
       <c r="W94" t="n">
-        <v>5330.300999999999</v>
+        <v>86.09999999999999</v>
       </c>
       <c r="X94" t="n">
-        <v>1040.26</v>
+        <v>16.6</v>
       </c>
     </row>
     <row r="95">
@@ -17674,22 +17674,22 @@
         <v>31069</v>
       </c>
       <c r="S95" t="n">
-        <v>6230.4223</v>
+        <v>87.43000000000001</v>
       </c>
       <c r="T95" t="n">
-        <v>50.26471</v>
+        <v>8.08</v>
       </c>
       <c r="U95" t="n">
-        <v>3340.323504999999</v>
+        <v>67.55500000000001</v>
       </c>
       <c r="V95" t="n">
-        <v>60.1505</v>
+        <v>7.55</v>
       </c>
       <c r="W95" t="n">
-        <v>5230.482300000001</v>
+        <v>78.03</v>
       </c>
       <c r="X95" t="n">
-        <v>1150.3006</v>
+        <v>28.06</v>
       </c>
     </row>
     <row r="96">
@@ -17762,22 +17762,22 @@
         <v>7815</v>
       </c>
       <c r="S96" t="n">
-        <v>12160.381408</v>
+        <v>139.948</v>
       </c>
       <c r="T96" t="n">
-        <v>10.172316</v>
+        <v>2.946</v>
       </c>
       <c r="U96" t="n">
-        <v>1120.282</v>
+        <v>25</v>
       </c>
       <c r="V96" t="n">
-        <v>10.0906</v>
+        <v>1.96</v>
       </c>
       <c r="W96" t="n">
-        <v>3370.2225</v>
+        <v>69.45</v>
       </c>
       <c r="X96" t="n">
-        <v>1150.3912</v>
+        <v>29.02</v>
       </c>
     </row>
     <row r="97">
@@ -17850,22 +17850,22 @@
         <v>10043</v>
       </c>
       <c r="S97" t="n">
-        <v>5140.3219</v>
+        <v>67.39</v>
       </c>
       <c r="T97" t="n">
-        <v>60.37260903</v>
+        <v>9.969299999999999</v>
       </c>
       <c r="U97" t="n">
-        <v>2260.2629</v>
+        <v>48.89</v>
       </c>
       <c r="V97" t="n">
-        <v>10.12</v>
+        <v>2.2</v>
       </c>
       <c r="W97" t="n">
-        <v>6330.330900000001</v>
+        <v>96.38999999999999</v>
       </c>
       <c r="X97" t="n">
-        <v>110.1818000902</v>
+        <v>12.98092</v>
       </c>
     </row>
     <row r="98">
@@ -17938,22 +17938,22 @@
         <v>2080</v>
       </c>
       <c r="S98" t="n">
-        <v>3140.210500000001</v>
+        <v>46.15000000000001</v>
       </c>
       <c r="T98" t="n">
-        <v>40.22260502</v>
+        <v>6.4652</v>
       </c>
       <c r="U98" t="n">
-        <v>4130.16120102</v>
+        <v>54.7212</v>
       </c>
       <c r="V98" t="n">
-        <v>0.0009</v>
+        <v>0.09</v>
       </c>
       <c r="W98" t="n">
-        <v>8270.449999999999</v>
+        <v>111.5</v>
       </c>
       <c r="X98" t="n">
-        <v>60.1905</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="99">
@@ -18026,22 +18026,22 @@
         <v>25525</v>
       </c>
       <c r="S99" t="n">
-        <v>13190.2811</v>
+        <v>151.91</v>
       </c>
       <c r="T99" t="n">
-        <v>20.32351</v>
+        <v>5.56</v>
       </c>
       <c r="U99" t="n">
-        <v>1280.3033</v>
+        <v>41.33000000000001</v>
       </c>
       <c r="V99" t="n">
         <v>0</v>
       </c>
       <c r="W99" t="n">
-        <v>2170.4018</v>
+        <v>41.18</v>
       </c>
       <c r="X99" t="n">
-        <v>130.4227</v>
+        <v>17.47</v>
       </c>
     </row>
     <row r="100">
@@ -18114,22 +18114,22 @@
         <v>42003</v>
       </c>
       <c r="S100" t="n">
-        <v>11240.2111</v>
+        <v>136.21</v>
       </c>
       <c r="T100" t="n">
-        <v>10.333603</v>
+        <v>4.663</v>
       </c>
       <c r="U100" t="n">
-        <v>2230.4022</v>
+        <v>47.22</v>
       </c>
       <c r="V100" t="n">
         <v>0</v>
       </c>
       <c r="W100" t="n">
-        <v>230.3423</v>
+        <v>26.63</v>
       </c>
       <c r="X100" t="n">
-        <v>60.43210000000001</v>
+        <v>10.51</v>
       </c>
     </row>
     <row r="101">
@@ -18202,22 +18202,22 @@
         <v>25479</v>
       </c>
       <c r="S101" t="n">
-        <v>6280.311900000001</v>
+        <v>91.28999999999999</v>
       </c>
       <c r="T101" t="n">
-        <v>4090.202412</v>
+        <v>51.252</v>
       </c>
       <c r="U101" t="n">
-        <v>2150.2907</v>
+        <v>37.97</v>
       </c>
       <c r="V101" t="n">
         <v>0</v>
       </c>
       <c r="W101" t="n">
-        <v>3320.3905</v>
+        <v>65.95</v>
       </c>
       <c r="X101" t="n">
-        <v>150.31</v>
+        <v>18.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>